<commit_message>
lisaa veikkauksia ja benzema muutokset
</commit_message>
<xml_diff>
--- a/Data/Lasse_Pasila_MM-Kisaveikkaus_2022.xlsx
+++ b/Data/Lasse_Pasila_MM-Kisaveikkaus_2022.xlsx
@@ -97,7 +97,7 @@
     <t xml:space="preserve">Ecuador</t>
   </si>
   <si>
-    <t xml:space="preserve">Karim Benzema</t>
+    <t xml:space="preserve">Kylian Mbappe</t>
   </si>
   <si>
     <t xml:space="preserve">Ranska</t>
@@ -297,7 +297,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d\.m\.;@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -372,6 +372,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -477,7 +483,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -558,11 +564,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -578,7 +588,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -586,7 +596,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -594,7 +604,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -627,10 +637,10 @@
   <dimension ref="A1:V126"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.54"/>
@@ -641,7 +651,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="2.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="2.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.55"/>
   </cols>
@@ -732,7 +742,7 @@
       <c r="U5" s="15"/>
       <c r="V5" s="15"/>
     </row>
-    <row r="6" s="15" customFormat="true" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="15" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
         <v>14</v>
       </c>
@@ -763,7 +773,7 @@
       <c r="K6" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="19" t="s">
+      <c r="N6" s="20" t="s">
         <v>18</v>
       </c>
       <c r="O6" s="19" t="s">
@@ -2046,173 +2056,173 @@
       <c r="I58" s="15"/>
       <c r="J58" s="15"/>
     </row>
-    <row r="59" s="20" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" s="21" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C59" s="21" t="s">
+      <c r="C59" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="F59" s="22" t="n">
+      <c r="F59" s="23" t="n">
         <v>12</v>
       </c>
-      <c r="G59" s="23"/>
-      <c r="H59" s="24"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="25"/>
     </row>
     <row r="60" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C60" s="25" t="s">
+      <c r="C60" s="26" t="s">
         <v>64</v>
       </c>
       <c r="F60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C61" s="25"/>
+      <c r="C61" s="26"/>
       <c r="F61" s="2"/>
     </row>
     <row r="62" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="26" t="s">
+      <c r="A62" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="B62" s="26"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="27"/>
-      <c r="E62" s="21"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="22"/>
       <c r="F62" s="2"/>
       <c r="I62" s="15"/>
       <c r="J62" s="15"/>
     </row>
     <row r="63" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F63" s="25"/>
-      <c r="G63" s="25"/>
-      <c r="H63" s="25"/>
+      <c r="F63" s="26"/>
+      <c r="G63" s="26"/>
+      <c r="H63" s="26"/>
       <c r="I63" s="15"/>
       <c r="J63" s="15"/>
     </row>
     <row r="64" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="28" t="s">
+      <c r="A64" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B64" s="28"/>
+      <c r="B64" s="29"/>
       <c r="F64" s="2"/>
       <c r="I64" s="15"/>
       <c r="J64" s="15"/>
     </row>
     <row r="65" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="28" t="s">
+      <c r="A65" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B65" s="28"/>
+      <c r="B65" s="29"/>
       <c r="J65" s="15"/>
     </row>
     <row r="66" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="28" t="s">
+      <c r="A66" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="B66" s="28"/>
-      <c r="F66" s="21"/>
-      <c r="G66" s="27"/>
-      <c r="H66" s="21"/>
+      <c r="B66" s="29"/>
+      <c r="F66" s="22"/>
+      <c r="G66" s="28"/>
+      <c r="H66" s="22"/>
       <c r="J66" s="15"/>
     </row>
     <row r="67" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="28"/>
-      <c r="B67" s="28"/>
+      <c r="A67" s="29"/>
+      <c r="B67" s="29"/>
       <c r="J67" s="15"/>
     </row>
     <row r="68" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="28" t="s">
+      <c r="A68" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="28"/>
+      <c r="B68" s="29"/>
       <c r="J68" s="15"/>
     </row>
     <row r="69" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="28" t="s">
+      <c r="A69" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="28"/>
+      <c r="B69" s="29"/>
       <c r="J69" s="15"/>
     </row>
     <row r="70" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="28" t="s">
+      <c r="A70" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="B70" s="28"/>
+      <c r="B70" s="29"/>
       <c r="J70" s="15"/>
     </row>
     <row r="71" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="28" t="s">
+      <c r="A71" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="B71" s="28"/>
+      <c r="B71" s="29"/>
       <c r="J71" s="15"/>
     </row>
     <row r="72" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="28"/>
-      <c r="B72" s="28"/>
+      <c r="A72" s="29"/>
+      <c r="B72" s="29"/>
       <c r="J72" s="15"/>
     </row>
     <row r="73" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="28" t="s">
+      <c r="A73" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="28"/>
+      <c r="B73" s="29"/>
       <c r="J73" s="15"/>
     </row>
     <row r="74" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="28"/>
-      <c r="B74" s="28"/>
+      <c r="A74" s="29"/>
+      <c r="B74" s="29"/>
       <c r="J74" s="15"/>
     </row>
     <row r="75" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="28" t="s">
+      <c r="A75" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="B75" s="28"/>
+      <c r="B75" s="29"/>
       <c r="J75" s="15"/>
     </row>
     <row r="76" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="28"/>
-      <c r="B76" s="28"/>
+      <c r="A76" s="29"/>
+      <c r="B76" s="29"/>
       <c r="J76" s="15"/>
     </row>
     <row r="77" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="28" t="s">
+      <c r="A77" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B77" s="28"/>
-      <c r="I77" s="29"/>
+      <c r="B77" s="29"/>
+      <c r="I77" s="30"/>
       <c r="J77" s="15"/>
     </row>
     <row r="78" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="28"/>
-      <c r="B78" s="28"/>
+      <c r="A78" s="29"/>
+      <c r="B78" s="29"/>
       <c r="J78" s="15"/>
     </row>
     <row r="79" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="28" t="s">
+      <c r="A79" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="B79" s="28"/>
+      <c r="B79" s="29"/>
       <c r="J79" s="15"/>
     </row>
     <row r="80" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="28"/>
-      <c r="B80" s="28"/>
+      <c r="A80" s="29"/>
+      <c r="B80" s="29"/>
       <c r="J80" s="15"/>
     </row>
     <row r="81" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="28" t="s">
+      <c r="A81" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="B81" s="28"/>
+      <c r="B81" s="29"/>
       <c r="J81" s="15"/>
     </row>
     <row r="82" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="29" t="s">
+      <c r="A82" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="B82" s="29"/>
+      <c r="B82" s="30"/>
     </row>
     <row r="83" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J83" s="15"/>
@@ -2222,19 +2232,19 @@
         <v>79</v>
       </c>
       <c r="B84" s="3"/>
-      <c r="C84" s="30"/>
-      <c r="D84" s="30" t="s">
+      <c r="C84" s="31"/>
+      <c r="D84" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="E84" s="30"/>
+      <c r="E84" s="31"/>
       <c r="J84" s="15"/>
     </row>
     <row r="85" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="3"/>
-      <c r="C85" s="30"/>
-      <c r="D85" s="31"/>
-      <c r="E85" s="30"/>
-      <c r="I85" s="20"/>
+      <c r="C85" s="31"/>
+      <c r="D85" s="32"/>
+      <c r="E85" s="31"/>
+      <c r="I85" s="21"/>
       <c r="J85" s="15"/>
     </row>
     <row r="86" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2244,58 +2254,58 @@
       <c r="B86" s="3"/>
     </row>
     <row r="87" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="30"/>
-      <c r="B87" s="30"/>
-      <c r="C87" s="30"/>
-      <c r="D87" s="30"/>
-      <c r="E87" s="30"/>
-      <c r="F87" s="31"/>
-      <c r="G87" s="30"/>
-      <c r="H87" s="30"/>
-      <c r="I87" s="20"/>
+      <c r="A87" s="31"/>
+      <c r="B87" s="31"/>
+      <c r="C87" s="31"/>
+      <c r="D87" s="31"/>
+      <c r="E87" s="31"/>
+      <c r="F87" s="32"/>
+      <c r="G87" s="31"/>
+      <c r="H87" s="31"/>
+      <c r="I87" s="21"/>
     </row>
     <row r="88" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J88" s="29"/>
-      <c r="K88" s="29"/>
-      <c r="L88" s="29"/>
+      <c r="J88" s="30"/>
+      <c r="K88" s="30"/>
+      <c r="L88" s="30"/>
     </row>
     <row r="97" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J97" s="20"/>
-      <c r="K97" s="20"/>
-      <c r="L97" s="20"/>
-    </row>
-    <row r="99" s="30" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J97" s="21"/>
+      <c r="K97" s="21"/>
+      <c r="L97" s="21"/>
+    </row>
+    <row r="99" s="31" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="D99" s="2"/>
       <c r="G99" s="2"/>
-      <c r="J99" s="20"/>
-      <c r="K99" s="20"/>
-      <c r="L99" s="20"/>
-    </row>
-    <row r="101" s="30" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J99" s="21"/>
+      <c r="K99" s="21"/>
+      <c r="L99" s="21"/>
+    </row>
+    <row r="101" s="31" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="D101" s="2"/>
       <c r="G101" s="2"/>
     </row>
     <row r="102" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J102" s="21"/>
-      <c r="K102" s="21"/>
-      <c r="L102" s="21"/>
+      <c r="J102" s="22"/>
+      <c r="K102" s="22"/>
+      <c r="L102" s="22"/>
     </row>
     <row r="103" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I103" s="30"/>
+      <c r="I103" s="31"/>
     </row>
     <row r="124" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J124" s="30"/>
-      <c r="K124" s="30"/>
-      <c r="L124" s="30"/>
+      <c r="J124" s="31"/>
+      <c r="K124" s="31"/>
+      <c r="L124" s="31"/>
     </row>
     <row r="126" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J126" s="30"/>
-      <c r="K126" s="30"/>
-      <c r="L126" s="30"/>
+      <c r="J126" s="31"/>
+      <c r="K126" s="31"/>
+      <c r="L126" s="31"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2322,7 +2332,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2345,7 +2355,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>